<commit_message>
Full system monitoring of PCB
</commit_message>
<xml_diff>
--- a/Hardware/UPD_PCB/Computations/buck_converter.xlsx
+++ b/Hardware/UPD_PCB/Computations/buck_converter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dries\Desktop\git\AI.R-ATV\Hardware\UPD_PCB\Computations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CACCE9-C4C7-4AC9-B995-8222F6F697B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20554F1-6733-46B0-9F59-D19579EA9BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{4B964BCB-4FB7-4901-A42B-2621AA10B7DC}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="25760" windowHeight="15440" xr2:uid="{4B964BCB-4FB7-4901-A42B-2621AA10B7DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>Vout</t>
   </si>
@@ -658,17 +658,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -680,6 +673,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,6 +693,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68202</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>536359</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>94291</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E780E4C-56BE-5861-9BD3-3D37214B945B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="678542" y="5687258"/>
+          <a:ext cx="5785511" cy="1943805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1014,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4220F6AD-D1C3-4C59-93DB-E2C5A9F2A0C6}">
-  <dimension ref="B1:T28"/>
+  <dimension ref="B1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="103" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1038,29 +1085,29 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="C2" s="27"/>
+      <c r="F2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="28"/>
-      <c r="J2" s="27" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="27"/>
+      <c r="J2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="28"/>
-      <c r="N2" s="27" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="27"/>
+      <c r="N2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28"/>
-      <c r="R2" s="27" t="s">
+      <c r="O2" s="31"/>
+      <c r="P2" s="27"/>
+      <c r="R2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="28"/>
+      <c r="S2" s="27"/>
       <c r="T2" s="21"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.35">
@@ -1250,11 +1297,11 @@
       </c>
     </row>
     <row r="8" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
@@ -1382,21 +1429,21 @@
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="28"/>
-      <c r="J15" s="31" t="s">
+      <c r="G15" s="31"/>
+      <c r="H15" s="27"/>
+      <c r="J15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="N15" s="27" t="s">
+      <c r="K15" s="29"/>
+      <c r="L15" s="30"/>
+      <c r="N15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="29"/>
-      <c r="P15" s="28"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
@@ -1613,111 +1660,126 @@
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="F25" s="30" t="s">
+    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F25" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="J25" s="30" t="s">
+      <c r="G25" s="31"/>
+      <c r="H25" s="27"/>
+      <c r="J25" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="N25" s="30" t="s">
+      <c r="K25" s="31"/>
+      <c r="L25" s="27"/>
+      <c r="N25" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="27"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="F26" t="s">
+      <c r="F26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="5">
         <v>2E-3</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="5">
         <v>45</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>3.5</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="2">
         <v>2.585</v>
       </c>
-      <c r="N27" t="s">
+      <c r="L27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O27">
-        <v>19</v>
-      </c>
-      <c r="P27" t="s">
+      <c r="O27" s="2">
+        <v>40</v>
+      </c>
+      <c r="P27" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="F28" t="s">
+    <row r="28" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F28" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="13">
         <f>G27/(2^15)</f>
         <v>1.068115234375E-4</v>
       </c>
-      <c r="J28" t="s">
+      <c r="H28" s="14"/>
+      <c r="J28" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="13">
         <f>(K27-(5.013/2))/0.045</f>
         <v>1.7444444444444449</v>
       </c>
-      <c r="N28" s="26" t="s">
+      <c r="L28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="13">
         <f>O27/O26</f>
-        <v>3800</v>
-      </c>
-      <c r="P28" t="s">
+        <v>8000</v>
+      </c>
+      <c r="P28" s="14" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K36" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="J25:L25"/>
     <mergeCell ref="B2:C2"/>
@@ -1725,19 +1787,23 @@
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="N25:P25"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="403a2287-8c7c-4a34-90c2-dbf3c4c1f054" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002223319B6B573345B80463C8BA005F6D" ma:contentTypeVersion="6" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="b41b03fd4873277aac50c366e6e24fb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="403a2287-8c7c-4a34-90c2-dbf3c4c1f054" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8639b9a5ca5a44d7a5aeb80dad9e886" ns3:_="">
     <xsd:import namespace="403a2287-8c7c-4a34-90c2-dbf3c4c1f054"/>
@@ -1893,14 +1959,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="403a2287-8c7c-4a34-90c2-dbf3c4c1f054" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1911,6 +1969,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7A3D88-0D14-4A68-A3DA-4E95883CF175}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="403a2287-8c7c-4a34-90c2-dbf3c4c1f054"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D2F193B-74DC-4E6D-9C0A-4D5F090DCF00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1928,22 +2002,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7A3D88-0D14-4A68-A3DA-4E95883CF175}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="403a2287-8c7c-4a34-90c2-dbf3c4c1f054"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0D6BF2D-DFAA-4729-8DDC-2D8D8E787D78}">
   <ds:schemaRefs>

</xml_diff>